<commit_message>
modifications to facebook ad processing
</commit_message>
<xml_diff>
--- a/temp/data_raw/facebook_profiles.xlsx
+++ b/temp/data_raw/facebook_profiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienberman/Documents/0-Thesis/temp/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E101C3D-C45D-3B46-9050-40CE00923FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D0D53-DF81-B045-BCA1-D149CCBBB6E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34240" yWindow="500" windowWidth="32240" windowHeight="21100" xr2:uid="{72EAA87E-7553-CE4F-BA02-73C64484A4D8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="818">
   <si>
     <t>name_first_last</t>
   </si>
@@ -1220,9 +1220,6 @@
     <t>page_id</t>
   </si>
   <si>
-    <t>FIX THIS</t>
-  </si>
-  <si>
     <t>page_id_2</t>
   </si>
   <si>
@@ -2009,12 +2006,6 @@
     <t>153080620724</t>
   </si>
   <si>
-    <t>325751000000</t>
-  </si>
-  <si>
-    <t>531624000000000</t>
-  </si>
-  <si>
     <t>122289898323229</t>
   </si>
   <si>
@@ -2472,6 +2463,33 @@
   </si>
   <si>
     <t>1626571454106828</t>
+  </si>
+  <si>
+    <t>52563647525</t>
+  </si>
+  <si>
+    <t>109592402468562</t>
+  </si>
+  <si>
+    <t>1490813904322906</t>
+  </si>
+  <si>
+    <t>100110638215668</t>
+  </si>
+  <si>
+    <t>213918568751224</t>
+  </si>
+  <si>
+    <t>1409012545881430</t>
+  </si>
+  <si>
+    <t>149366465128820</t>
+  </si>
+  <si>
+    <t>104346771140701</t>
+  </si>
+  <si>
+    <t>191055010919565</t>
   </si>
 </sst>
 </file>
@@ -2864,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD12365-70E5-7F49-9FE3-1BEA6068403D}">
   <dimension ref="A1:C393"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A354" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D377" sqref="D377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,7 +2903,7 @@
         <v>393</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2893,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -2902,7 +2920,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2911,7 +2929,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -2920,7 +2938,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -2929,7 +2947,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -2938,7 +2956,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -2947,7 +2965,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="C8" s="2"/>
     </row>
@@ -2956,7 +2974,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -2965,7 +2983,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -2974,7 +2992,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -2983,7 +3001,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -2992,7 +3010,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -3001,7 +3019,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -3010,7 +3028,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -3019,7 +3037,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -3028,7 +3046,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C17" s="2"/>
     </row>
@@ -3037,7 +3055,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -3046,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="C19" s="2"/>
     </row>
@@ -3055,7 +3073,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="C20" s="2"/>
     </row>
@@ -3076,7 +3094,7 @@
         <v>13063797831</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3084,7 +3102,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="C23" s="2"/>
     </row>
@@ -3093,7 +3111,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C24" s="3"/>
     </row>
@@ -3102,7 +3120,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="C25" s="2"/>
     </row>
@@ -3111,7 +3129,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -3120,7 +3138,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C27" s="2"/>
     </row>
@@ -3129,7 +3147,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -3138,7 +3156,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C29" s="2"/>
     </row>
@@ -3147,7 +3165,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="C30" s="2"/>
     </row>
@@ -3156,10 +3174,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -3167,7 +3185,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="C32" s="2"/>
     </row>
@@ -3176,7 +3194,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="C33" s="2"/>
     </row>
@@ -3185,7 +3203,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -3194,7 +3212,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="C35" s="2"/>
     </row>
@@ -3203,7 +3221,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="C36" s="2"/>
     </row>
@@ -3212,7 +3230,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C37" s="2"/>
     </row>
@@ -3221,7 +3239,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="C38" s="2"/>
     </row>
@@ -3230,7 +3248,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -3239,7 +3257,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C40" s="2"/>
     </row>
@@ -3248,7 +3266,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="C41" s="2"/>
     </row>
@@ -3257,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="C42" s="2"/>
     </row>
@@ -3266,7 +3284,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="C43" s="2"/>
     </row>
@@ -3275,7 +3293,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="C44" s="2"/>
     </row>
@@ -3284,7 +3302,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C45" s="2"/>
     </row>
@@ -3293,7 +3311,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
       <c r="C46" s="2"/>
     </row>
@@ -3302,7 +3320,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="C47" s="2"/>
     </row>
@@ -3311,7 +3329,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C48" s="2"/>
     </row>
@@ -3320,7 +3338,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C49" s="2"/>
     </row>
@@ -3329,7 +3347,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>394</v>
+        <v>813</v>
       </c>
       <c r="C50" s="2"/>
     </row>
@@ -3338,7 +3356,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="C51" s="2"/>
     </row>
@@ -3347,7 +3365,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="C52" s="2"/>
     </row>
@@ -3356,7 +3374,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="C53" s="2"/>
     </row>
@@ -3365,7 +3383,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="C54" s="2"/>
     </row>
@@ -3374,7 +3392,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="C55" s="2"/>
     </row>
@@ -3383,7 +3401,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="C56" s="2"/>
     </row>
@@ -3392,7 +3410,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="C57" s="2"/>
     </row>
@@ -3401,7 +3419,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="C58" s="2"/>
     </row>
@@ -3410,7 +3428,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="C59" s="2"/>
     </row>
@@ -3419,7 +3437,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="C60" s="2"/>
     </row>
@@ -3428,7 +3446,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C61" s="2"/>
     </row>
@@ -3437,7 +3455,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C62" s="2"/>
     </row>
@@ -3446,7 +3464,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C63" s="2"/>
     </row>
@@ -3455,7 +3473,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C64" s="2"/>
     </row>
@@ -3464,7 +3482,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C65" s="2"/>
     </row>
@@ -3473,7 +3491,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="C66" s="2"/>
     </row>
@@ -3482,7 +3500,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="C67" s="2"/>
     </row>
@@ -3491,7 +3509,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C68" s="2"/>
     </row>
@@ -3500,7 +3518,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C69" s="2"/>
     </row>
@@ -3509,7 +3527,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C70" s="2"/>
     </row>
@@ -3518,7 +3536,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -3527,7 +3545,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C72" s="2"/>
     </row>
@@ -3536,7 +3554,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C73" s="2"/>
     </row>
@@ -3545,7 +3563,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="C74" s="2"/>
     </row>
@@ -3554,7 +3572,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="C75" s="2"/>
     </row>
@@ -3563,7 +3581,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C76" s="2"/>
     </row>
@@ -3572,7 +3590,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="C77" s="2"/>
     </row>
@@ -3581,7 +3599,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="C78" s="2"/>
     </row>
@@ -3590,7 +3608,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="C79" s="2"/>
     </row>
@@ -3599,7 +3617,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C80" s="2"/>
     </row>
@@ -3608,7 +3626,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C81" s="2"/>
     </row>
@@ -3617,7 +3635,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="C82" s="2"/>
     </row>
@@ -3626,10 +3644,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -3637,7 +3655,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="C84" s="2"/>
     </row>
@@ -3646,7 +3664,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C85" s="2"/>
     </row>
@@ -3655,7 +3673,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C86" s="2"/>
     </row>
@@ -3664,7 +3682,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="C87" s="2"/>
     </row>
@@ -3673,7 +3691,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="C88" s="2"/>
     </row>
@@ -3682,7 +3700,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="C89" s="2"/>
     </row>
@@ -3691,7 +3709,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C90" s="2"/>
     </row>
@@ -3700,7 +3718,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="C91" s="2"/>
     </row>
@@ -3709,7 +3727,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="C92" s="2"/>
     </row>
@@ -3718,7 +3736,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="C93" s="2"/>
     </row>
@@ -3727,7 +3745,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C94" s="2"/>
     </row>
@@ -3736,7 +3754,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="C95" s="2"/>
     </row>
@@ -3745,7 +3763,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="C96" s="2"/>
     </row>
@@ -3754,37 +3772,37 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>657</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2" t="s">
-        <v>658</v>
-      </c>
+      <c r="B98" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="4"/>
+      <c r="B100" s="4" t="s">
+        <v>811</v>
+      </c>
       <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -3792,7 +3810,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C101" s="2"/>
     </row>
@@ -3801,7 +3819,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C102" s="2"/>
     </row>
@@ -3810,7 +3828,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C103" s="2"/>
     </row>
@@ -3819,7 +3837,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C104" s="2"/>
     </row>
@@ -3828,10 +3846,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -3839,7 +3857,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C106" s="2"/>
     </row>
@@ -3848,7 +3866,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C107" s="2"/>
     </row>
@@ -3857,7 +3875,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C108" s="2"/>
     </row>
@@ -3866,7 +3884,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C109" s="2"/>
     </row>
@@ -3875,10 +3893,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -3886,7 +3904,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C111" s="2"/>
     </row>
@@ -3895,7 +3913,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C112" s="2"/>
     </row>
@@ -3904,7 +3922,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C113" s="2"/>
     </row>
@@ -3913,7 +3931,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C114" s="2"/>
     </row>
@@ -3922,7 +3940,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C115" s="2"/>
     </row>
@@ -3931,7 +3949,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C116" s="2"/>
     </row>
@@ -3940,10 +3958,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -3951,7 +3969,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C118" s="2"/>
     </row>
@@ -3960,10 +3978,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -3971,10 +3989,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -3982,7 +4000,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C121" s="2"/>
     </row>
@@ -3991,7 +4009,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C122" s="2"/>
     </row>
@@ -4000,7 +4018,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C123" s="2"/>
     </row>
@@ -4009,7 +4027,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C124" s="2"/>
     </row>
@@ -4018,7 +4036,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C125" s="2"/>
     </row>
@@ -4027,7 +4045,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C126" s="2"/>
     </row>
@@ -4036,7 +4054,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C127" s="2"/>
     </row>
@@ -4045,7 +4063,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C128" s="2"/>
     </row>
@@ -4054,10 +4072,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
@@ -4065,7 +4083,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C130" s="2"/>
     </row>
@@ -4074,10 +4092,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
@@ -4085,7 +4103,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C132" s="2"/>
     </row>
@@ -4094,7 +4112,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C133" s="2"/>
     </row>
@@ -4103,7 +4121,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C134" s="2"/>
     </row>
@@ -4112,7 +4130,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C135" s="2"/>
     </row>
@@ -4121,10 +4139,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
@@ -4132,7 +4150,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C137" s="2"/>
     </row>
@@ -4141,7 +4159,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C138" s="2"/>
     </row>
@@ -4150,10 +4168,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
@@ -4161,7 +4179,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C140" s="2"/>
     </row>
@@ -4170,10 +4188,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
@@ -4181,7 +4199,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C142" s="2"/>
     </row>
@@ -4190,10 +4208,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
@@ -4201,7 +4219,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C144" s="2"/>
     </row>
@@ -4210,7 +4228,7 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C145" s="2"/>
     </row>
@@ -4219,10 +4237,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
@@ -4230,7 +4248,7 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C147" s="2"/>
     </row>
@@ -4239,10 +4257,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
@@ -4250,7 +4268,7 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C149" s="2"/>
     </row>
@@ -4259,7 +4277,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C150" s="2"/>
     </row>
@@ -4268,7 +4286,7 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C151" s="2"/>
     </row>
@@ -4277,7 +4295,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C152" s="2"/>
     </row>
@@ -4286,7 +4304,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C153" s="2"/>
     </row>
@@ -4295,7 +4313,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C154" s="2"/>
     </row>
@@ -4304,10 +4322,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
@@ -4315,7 +4333,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C156" s="2"/>
     </row>
@@ -4324,7 +4342,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C157" s="2"/>
     </row>
@@ -4333,7 +4351,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C158" s="2"/>
     </row>
@@ -4342,7 +4360,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="C159" s="2"/>
     </row>
@@ -4351,7 +4369,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C160" s="2"/>
     </row>
@@ -4360,7 +4378,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C161" s="2"/>
     </row>
@@ -4369,10 +4387,10 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
@@ -4380,7 +4398,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C163" s="2"/>
     </row>
@@ -4389,7 +4407,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C164" s="2"/>
     </row>
@@ -4398,7 +4416,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="C165" s="2"/>
     </row>
@@ -4407,7 +4425,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C166" s="2"/>
     </row>
@@ -4416,7 +4434,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C167" s="2"/>
     </row>
@@ -4425,10 +4443,10 @@
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
@@ -4436,7 +4454,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C169" s="2"/>
     </row>
@@ -4445,7 +4463,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C170" s="2"/>
     </row>
@@ -4454,10 +4472,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
@@ -4465,7 +4483,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="C172" s="2"/>
     </row>
@@ -4474,7 +4492,7 @@
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C173" s="2"/>
     </row>
@@ -4483,7 +4501,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C174" s="2"/>
     </row>
@@ -4492,7 +4510,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="C175" s="2"/>
     </row>
@@ -4501,7 +4519,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="C176" s="2"/>
     </row>
@@ -4510,7 +4528,7 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C177" s="2"/>
     </row>
@@ -4519,7 +4537,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C178" s="2"/>
     </row>
@@ -4528,7 +4546,7 @@
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C179" s="2"/>
     </row>
@@ -4537,7 +4555,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C180" s="2"/>
     </row>
@@ -4546,7 +4564,7 @@
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C181" s="2"/>
     </row>
@@ -4555,7 +4573,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C182" s="2"/>
     </row>
@@ -4564,10 +4582,10 @@
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
@@ -4575,7 +4593,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C184" s="2"/>
     </row>
@@ -4584,7 +4602,7 @@
         <v>184</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C185" s="2"/>
     </row>
@@ -4593,7 +4611,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C186" s="2"/>
     </row>
@@ -4602,7 +4620,7 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C187" s="2"/>
     </row>
@@ -4611,7 +4629,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C188" s="2"/>
     </row>
@@ -4620,7 +4638,7 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C189" s="2"/>
     </row>
@@ -4629,7 +4647,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C190" s="2"/>
     </row>
@@ -4638,7 +4656,7 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C191" s="2"/>
     </row>
@@ -4647,7 +4665,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C192" s="2"/>
     </row>
@@ -4656,7 +4674,7 @@
         <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="C193" s="2"/>
     </row>
@@ -4665,7 +4683,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="C194" s="2"/>
     </row>
@@ -4674,7 +4692,7 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C195" s="2"/>
     </row>
@@ -4683,7 +4701,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C196" s="2"/>
     </row>
@@ -4692,7 +4710,7 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C197" s="2"/>
     </row>
@@ -4701,7 +4719,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C198" s="2"/>
     </row>
@@ -4710,7 +4728,7 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C199" s="2"/>
     </row>
@@ -4719,7 +4737,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C200" s="2"/>
     </row>
@@ -4728,7 +4746,7 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="C201" s="2"/>
     </row>
@@ -4737,7 +4755,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C202" s="2"/>
     </row>
@@ -4746,7 +4764,7 @@
         <v>202</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C203" s="2"/>
     </row>
@@ -4755,7 +4773,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C204" s="2"/>
     </row>
@@ -4764,10 +4782,10 @@
         <v>204</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
@@ -4775,7 +4793,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C206" s="2"/>
     </row>
@@ -4784,7 +4802,7 @@
         <v>206</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="C207" s="2"/>
     </row>
@@ -4793,7 +4811,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="C208" s="2"/>
     </row>
@@ -4802,7 +4820,7 @@
         <v>208</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C209" s="2"/>
     </row>
@@ -4811,7 +4829,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C210" s="2"/>
     </row>
@@ -4820,7 +4838,7 @@
         <v>210</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C211" s="2"/>
     </row>
@@ -4829,7 +4847,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C212" s="2"/>
     </row>
@@ -4838,7 +4856,7 @@
         <v>212</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>394</v>
+        <v>817</v>
       </c>
       <c r="C213" s="2"/>
     </row>
@@ -4847,7 +4865,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C214" s="2"/>
     </row>
@@ -4856,10 +4874,10 @@
         <v>214</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
@@ -4867,7 +4885,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C216" s="2"/>
     </row>
@@ -4876,7 +4894,7 @@
         <v>216</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C217" s="2"/>
     </row>
@@ -4885,10 +4903,10 @@
         <v>217</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
@@ -4896,7 +4914,7 @@
         <v>218</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C219" s="2"/>
     </row>
@@ -4905,18 +4923,16 @@
         <v>219</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>394</v>
-      </c>
+        <v>562</v>
+      </c>
+      <c r="C220" s="2"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="2" t="s">
         <v>220</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C221" s="2"/>
     </row>
@@ -4925,7 +4941,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C222" s="2"/>
     </row>
@@ -4934,7 +4950,7 @@
         <v>222</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C223" s="2"/>
     </row>
@@ -4943,7 +4959,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>394</v>
+        <v>816</v>
       </c>
       <c r="C224" s="2"/>
     </row>
@@ -4952,7 +4968,7 @@
         <v>224</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C225" s="2"/>
     </row>
@@ -4961,7 +4977,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C226" s="2"/>
     </row>
@@ -4970,7 +4986,7 @@
         <v>226</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C227" s="2"/>
     </row>
@@ -4979,7 +4995,7 @@
         <v>227</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C228" s="2"/>
     </row>
@@ -4988,7 +5004,7 @@
         <v>228</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C229" s="2"/>
     </row>
@@ -4997,7 +5013,7 @@
         <v>229</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C230" s="2"/>
     </row>
@@ -5006,7 +5022,7 @@
         <v>230</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>394</v>
+        <v>809</v>
       </c>
       <c r="C231" s="2"/>
     </row>
@@ -5015,7 +5031,7 @@
         <v>231</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C232" s="2"/>
     </row>
@@ -5024,7 +5040,7 @@
         <v>232</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C233" s="2"/>
     </row>
@@ -5033,7 +5049,7 @@
         <v>233</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C234" s="2"/>
     </row>
@@ -5042,7 +5058,7 @@
         <v>234</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C235" s="2"/>
     </row>
@@ -5051,7 +5067,7 @@
         <v>235</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C236" s="2"/>
     </row>
@@ -5060,7 +5076,7 @@
         <v>236</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C237" s="2"/>
     </row>
@@ -5069,7 +5085,7 @@
         <v>237</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C238" s="2"/>
     </row>
@@ -5078,7 +5094,7 @@
         <v>238</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C239" s="2"/>
     </row>
@@ -5087,7 +5103,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C240" s="2"/>
     </row>
@@ -5096,7 +5112,7 @@
         <v>240</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C241" s="2"/>
     </row>
@@ -5105,7 +5121,7 @@
         <v>241</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C242" s="2"/>
     </row>
@@ -5114,10 +5130,10 @@
         <v>242</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
@@ -5125,7 +5141,7 @@
         <v>243</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="C244" s="2"/>
     </row>
@@ -5134,7 +5150,7 @@
         <v>244</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C245" s="2"/>
     </row>
@@ -5143,7 +5159,7 @@
         <v>245</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C246" s="2"/>
     </row>
@@ -5152,7 +5168,7 @@
         <v>246</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C247" s="2"/>
     </row>
@@ -5161,7 +5177,7 @@
         <v>247</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C248" s="2"/>
     </row>
@@ -5170,7 +5186,7 @@
         <v>248</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C249" s="2"/>
     </row>
@@ -5179,7 +5195,7 @@
         <v>249</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C250" s="2"/>
     </row>
@@ -5188,7 +5204,7 @@
         <v>250</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C251" s="2"/>
     </row>
@@ -5197,7 +5213,7 @@
         <v>251</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C252" s="2"/>
     </row>
@@ -5206,10 +5222,10 @@
         <v>252</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
@@ -5217,7 +5233,7 @@
         <v>253</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C254" s="2"/>
     </row>
@@ -5226,7 +5242,7 @@
         <v>254</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C255" s="2"/>
     </row>
@@ -5235,7 +5251,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="C256" s="2"/>
     </row>
@@ -5244,7 +5260,7 @@
         <v>256</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C257" s="2"/>
     </row>
@@ -5253,7 +5269,7 @@
         <v>257</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C258" s="2"/>
     </row>
@@ -5262,7 +5278,7 @@
         <v>258</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C259" s="2"/>
     </row>
@@ -5271,7 +5287,7 @@
         <v>259</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C260" s="2"/>
     </row>
@@ -5280,7 +5296,7 @@
         <v>260</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C261" s="2"/>
     </row>
@@ -5289,7 +5305,7 @@
         <v>261</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C262" s="2"/>
     </row>
@@ -5298,7 +5314,7 @@
         <v>262</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C263" s="2"/>
     </row>
@@ -5307,7 +5323,7 @@
         <v>263</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C264" s="2"/>
     </row>
@@ -5316,7 +5332,7 @@
         <v>264</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C265" s="2"/>
     </row>
@@ -5325,7 +5341,7 @@
         <v>265</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="C266" s="2"/>
     </row>
@@ -5334,7 +5350,7 @@
         <v>266</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C267" s="2"/>
     </row>
@@ -5343,7 +5359,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="C268" s="2"/>
     </row>
@@ -5352,7 +5368,7 @@
         <v>268</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>394</v>
+        <v>814</v>
       </c>
       <c r="C269" s="2"/>
     </row>
@@ -5361,7 +5377,7 @@
         <v>269</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C270" s="2"/>
     </row>
@@ -5370,10 +5386,10 @@
         <v>270</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
@@ -5381,7 +5397,7 @@
         <v>271</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C272" s="2"/>
     </row>
@@ -5390,7 +5406,7 @@
         <v>272</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C273" s="2"/>
     </row>
@@ -5399,7 +5415,7 @@
         <v>273</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C274" s="2"/>
     </row>
@@ -5408,7 +5424,7 @@
         <v>274</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C275" s="2"/>
     </row>
@@ -5417,7 +5433,7 @@
         <v>275</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C276" s="2"/>
     </row>
@@ -5426,7 +5442,7 @@
         <v>276</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C277" s="2"/>
     </row>
@@ -5435,7 +5451,7 @@
         <v>277</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C278" s="2"/>
     </row>
@@ -5444,7 +5460,7 @@
         <v>278</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C279" s="2"/>
     </row>
@@ -5453,7 +5469,7 @@
         <v>279</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C280" s="2"/>
     </row>
@@ -5462,7 +5478,7 @@
         <v>280</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C281" s="2"/>
     </row>
@@ -5471,7 +5487,7 @@
         <v>281</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C282" s="2"/>
     </row>
@@ -5480,7 +5496,7 @@
         <v>282</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C283" s="2"/>
     </row>
@@ -5489,7 +5505,7 @@
         <v>283</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C284" s="2"/>
     </row>
@@ -5498,10 +5514,10 @@
         <v>284</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
@@ -5509,7 +5525,7 @@
         <v>285</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="C286" s="2"/>
     </row>
@@ -5518,10 +5534,10 @@
         <v>286</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
@@ -5529,7 +5545,7 @@
         <v>287</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C288" s="2"/>
     </row>
@@ -5538,7 +5554,7 @@
         <v>288</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C289" s="2"/>
     </row>
@@ -5547,7 +5563,7 @@
         <v>289</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C290" s="2"/>
     </row>
@@ -5556,7 +5572,7 @@
         <v>290</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C291" s="2"/>
     </row>
@@ -5565,7 +5581,7 @@
         <v>291</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C292" s="2"/>
     </row>
@@ -5574,7 +5590,7 @@
         <v>292</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="C293" s="2"/>
     </row>
@@ -5583,7 +5599,7 @@
         <v>293</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C294" s="2"/>
     </row>
@@ -5592,7 +5608,7 @@
         <v>294</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="C295" s="2"/>
     </row>
@@ -5601,7 +5617,7 @@
         <v>295</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C296" s="2"/>
     </row>
@@ -5610,7 +5626,7 @@
         <v>296</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C297" s="2"/>
     </row>
@@ -5619,7 +5635,7 @@
         <v>297</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>394</v>
+        <v>815</v>
       </c>
       <c r="C298" s="2"/>
     </row>
@@ -5628,7 +5644,7 @@
         <v>298</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C299" s="2"/>
     </row>
@@ -5637,7 +5653,7 @@
         <v>299</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C300" s="2"/>
     </row>
@@ -5646,7 +5662,7 @@
         <v>300</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C301" s="2"/>
     </row>
@@ -5655,7 +5671,7 @@
         <v>301</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C302" s="2"/>
     </row>
@@ -5664,7 +5680,7 @@
         <v>302</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C303" s="2"/>
     </row>
@@ -5673,7 +5689,7 @@
         <v>303</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C304" s="2"/>
     </row>
@@ -5682,7 +5698,7 @@
         <v>304</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C305" s="2"/>
     </row>
@@ -5691,7 +5707,7 @@
         <v>305</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C306" s="2"/>
     </row>
@@ -5700,7 +5716,7 @@
         <v>306</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C307" s="2"/>
     </row>
@@ -5709,7 +5725,7 @@
         <v>307</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C308" s="2"/>
     </row>
@@ -5718,7 +5734,7 @@
         <v>308</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C309" s="2"/>
     </row>
@@ -5727,7 +5743,7 @@
         <v>309</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C310" s="2"/>
     </row>
@@ -5736,7 +5752,7 @@
         <v>310</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C311" s="2"/>
     </row>
@@ -5745,7 +5761,7 @@
         <v>311</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C312" s="2"/>
     </row>
@@ -5754,7 +5770,7 @@
         <v>312</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C313" s="2"/>
     </row>
@@ -5763,7 +5779,7 @@
         <v>313</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C314" s="2"/>
     </row>
@@ -5772,7 +5788,7 @@
         <v>314</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C315" s="2"/>
     </row>
@@ -5781,7 +5797,7 @@
         <v>315</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C316" s="2"/>
     </row>
@@ -5790,7 +5806,7 @@
         <v>316</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C317" s="2"/>
     </row>
@@ -5799,7 +5815,7 @@
         <v>317</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C318" s="2"/>
     </row>
@@ -5808,7 +5824,7 @@
         <v>318</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C319" s="2"/>
     </row>
@@ -5817,7 +5833,7 @@
         <v>319</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C320" s="2"/>
     </row>
@@ -5826,7 +5842,7 @@
         <v>320</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C321" s="2"/>
     </row>
@@ -5835,7 +5851,7 @@
         <v>321</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C322" s="2"/>
     </row>
@@ -5844,7 +5860,7 @@
         <v>322</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C323" s="2"/>
     </row>
@@ -5853,7 +5869,7 @@
         <v>323</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C324" s="2"/>
     </row>
@@ -5862,10 +5878,10 @@
         <v>324</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C325" s="2" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
@@ -5873,7 +5889,7 @@
         <v>325</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C326" s="2"/>
     </row>
@@ -5882,7 +5898,7 @@
         <v>326</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C327" s="2"/>
     </row>
@@ -5891,7 +5907,7 @@
         <v>327</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C328" s="2"/>
     </row>
@@ -5900,7 +5916,7 @@
         <v>328</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C329" s="2"/>
     </row>
@@ -5909,7 +5925,7 @@
         <v>329</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C330" s="2"/>
     </row>
@@ -5918,7 +5934,7 @@
         <v>330</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C331" s="2"/>
     </row>
@@ -5927,7 +5943,7 @@
         <v>331</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="C332" s="2"/>
     </row>
@@ -5936,7 +5952,7 @@
         <v>332</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="C333" s="2"/>
     </row>
@@ -5945,7 +5961,7 @@
         <v>333</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="C334" s="2"/>
     </row>
@@ -5954,7 +5970,7 @@
         <v>334</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="C335" s="2"/>
     </row>
@@ -5963,7 +5979,7 @@
         <v>335</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="C336" s="2"/>
     </row>
@@ -5972,7 +5988,7 @@
         <v>336</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C337" s="2"/>
     </row>
@@ -5981,7 +5997,7 @@
         <v>337</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C338" s="2"/>
     </row>
@@ -5990,7 +6006,7 @@
         <v>338</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C339" s="2"/>
     </row>
@@ -5999,7 +6015,7 @@
         <v>339</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C340" s="2"/>
     </row>
@@ -6008,7 +6024,7 @@
         <v>340</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C341" s="2"/>
     </row>
@@ -6017,7 +6033,7 @@
         <v>341</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C342" s="2"/>
     </row>
@@ -6026,7 +6042,7 @@
         <v>342</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C343" s="2"/>
     </row>
@@ -6035,7 +6051,7 @@
         <v>343</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>394</v>
+        <v>812</v>
       </c>
       <c r="C344" s="2"/>
     </row>
@@ -6044,7 +6060,7 @@
         <v>344</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C345" s="2"/>
     </row>
@@ -6053,7 +6069,7 @@
         <v>345</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C346" s="2"/>
     </row>
@@ -6062,7 +6078,7 @@
         <v>346</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C347" s="2"/>
     </row>
@@ -6071,7 +6087,7 @@
         <v>347</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="C348" s="2"/>
     </row>
@@ -6080,7 +6096,7 @@
         <v>348</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C349" s="2"/>
     </row>
@@ -6089,7 +6105,7 @@
         <v>349</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C350" s="2"/>
     </row>
@@ -6098,7 +6114,7 @@
         <v>350</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C351" s="2"/>
     </row>
@@ -6107,7 +6123,7 @@
         <v>351</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C352" s="2"/>
     </row>
@@ -6116,7 +6132,7 @@
         <v>352</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="C353" s="2"/>
     </row>
@@ -6125,7 +6141,7 @@
         <v>353</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C354" s="2"/>
     </row>
@@ -6134,7 +6150,7 @@
         <v>354</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C355" s="2"/>
     </row>
@@ -6143,7 +6159,7 @@
         <v>355</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C356" s="2"/>
     </row>
@@ -6152,7 +6168,7 @@
         <v>356</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C357" s="2"/>
     </row>
@@ -6161,7 +6177,7 @@
         <v>357</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C358" s="2"/>
     </row>
@@ -6170,10 +6186,10 @@
         <v>358</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
@@ -6181,7 +6197,7 @@
         <v>359</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C360" s="2"/>
     </row>
@@ -6190,7 +6206,7 @@
         <v>360</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="C361" s="2"/>
     </row>
@@ -6199,7 +6215,7 @@
         <v>361</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C362" s="2"/>
     </row>
@@ -6208,7 +6224,7 @@
         <v>362</v>
       </c>
       <c r="B363" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C363" s="2"/>
     </row>
@@ -6217,7 +6233,7 @@
         <v>363</v>
       </c>
       <c r="B364" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C364" s="2"/>
     </row>
@@ -6226,7 +6242,7 @@
         <v>364</v>
       </c>
       <c r="B365" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C365" s="2"/>
     </row>
@@ -6235,7 +6251,7 @@
         <v>365</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C366" s="2"/>
     </row>
@@ -6244,7 +6260,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="2" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C367" s="2"/>
     </row>
@@ -6253,7 +6269,7 @@
         <v>367</v>
       </c>
       <c r="B368" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C368" s="2"/>
     </row>
@@ -6262,7 +6278,7 @@
         <v>368</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="C369" s="2"/>
     </row>
@@ -6271,7 +6287,7 @@
         <v>369</v>
       </c>
       <c r="B370" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C370" s="2"/>
     </row>
@@ -6280,7 +6296,7 @@
         <v>370</v>
       </c>
       <c r="B371" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C371" s="2"/>
     </row>
@@ -6289,7 +6305,7 @@
         <v>371</v>
       </c>
       <c r="B372" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C372" s="2"/>
     </row>
@@ -6298,7 +6314,7 @@
         <v>372</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C373" s="2"/>
     </row>
@@ -6307,7 +6323,7 @@
         <v>373</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C374" s="2"/>
     </row>
@@ -6316,7 +6332,7 @@
         <v>374</v>
       </c>
       <c r="B375" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C375" s="2"/>
     </row>
@@ -6325,7 +6341,7 @@
         <v>375</v>
       </c>
       <c r="B376" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C376" s="2"/>
     </row>
@@ -6334,7 +6350,7 @@
         <v>376</v>
       </c>
       <c r="B377" s="2" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="C377" s="2"/>
     </row>
@@ -6343,7 +6359,7 @@
         <v>377</v>
       </c>
       <c r="B378" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C378" s="2"/>
     </row>
@@ -6352,7 +6368,7 @@
         <v>378</v>
       </c>
       <c r="B379" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C379" s="2"/>
     </row>
@@ -6361,7 +6377,7 @@
         <v>379</v>
       </c>
       <c r="B380" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C380" s="2"/>
     </row>
@@ -6370,7 +6386,7 @@
         <v>380</v>
       </c>
       <c r="B381" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C381" s="2"/>
     </row>
@@ -6379,7 +6395,7 @@
         <v>381</v>
       </c>
       <c r="B382" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C382" s="2"/>
     </row>
@@ -6388,7 +6404,7 @@
         <v>382</v>
       </c>
       <c r="B383" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C383" s="2"/>
     </row>
@@ -6397,7 +6413,7 @@
         <v>383</v>
       </c>
       <c r="B384" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C384" s="2"/>
     </row>
@@ -6406,7 +6422,7 @@
         <v>384</v>
       </c>
       <c r="B385" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C385" s="2"/>
     </row>
@@ -6415,10 +6431,10 @@
         <v>385</v>
       </c>
       <c r="B386" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C386" s="2" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.2">
@@ -6426,7 +6442,7 @@
         <v>386</v>
       </c>
       <c r="B387" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C387" s="2"/>
     </row>
@@ -6435,7 +6451,7 @@
         <v>387</v>
       </c>
       <c r="B388" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C388" s="2"/>
     </row>
@@ -6444,7 +6460,7 @@
         <v>388</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C389" s="2"/>
     </row>
@@ -6453,7 +6469,7 @@
         <v>389</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="C390" s="2"/>
     </row>
@@ -6462,7 +6478,7 @@
         <v>390</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C391" s="2"/>
     </row>
@@ -6471,7 +6487,7 @@
         <v>391</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C392" s="2"/>
     </row>
@@ -6480,7 +6496,7 @@
         <v>392</v>
       </c>
       <c r="B393" s="2" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C393" s="2"/>
     </row>

</xml_diff>